<commit_message>
commit new changed bg, and made it look cool
</commit_message>
<xml_diff>
--- a/recommended_cars.xlsx
+++ b/recommended_cars.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -58,43 +58,49 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Mercedes-Benz SLK-Class 55 AMG</t>
-  </si>
-  <si>
-    <t>Mercedes-Benz SL-Class SL 500</t>
-  </si>
-  <si>
-    <t>Mercedes-Benz S Class 2005 2013 S 500</t>
-  </si>
-  <si>
-    <t>Mercedes-Benz S Class 2005 2013 S 350 L</t>
-  </si>
-  <si>
-    <t>MercedesBenz</t>
-  </si>
-  <si>
-    <t>Bangalore</t>
+    <t>Tata Indigo eCS eLS BS IV</t>
+  </si>
+  <si>
+    <t>Tata Tiago 1.2 Revotron XT Option</t>
+  </si>
+  <si>
+    <t>Tata Indica Vista Quadrajet LS</t>
+  </si>
+  <si>
+    <t>Tata Indigo GLE</t>
+  </si>
+  <si>
+    <t>Tata Indigo LS Dicor</t>
+  </si>
+  <si>
+    <t>Tata</t>
   </si>
   <si>
     <t>Kolkata</t>
   </si>
   <si>
-    <t>Mumbai</t>
+    <t>Coimbatore</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>Diesel</t>
   </si>
   <si>
     <t>Petrol</t>
   </si>
   <si>
-    <t>Automatic</t>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>First</t>
   </si>
   <si>
     <t>Second</t>
-  </si>
-  <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>Third</t>
   </si>
 </sst>
 </file>
@@ -504,222 +510,222 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2">
-        <v>4691</v>
+        <v>3011</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="F2">
-        <v>3000</v>
+        <v>78000</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="J2">
-        <v>5461</v>
+        <v>1396</v>
       </c>
       <c r="K2">
-        <v>421</v>
+        <v>69.01000000000001</v>
       </c>
       <c r="L2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M2">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="N2">
-        <v>90</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3">
-        <v>4722</v>
+        <v>4748</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3">
-        <v>2010</v>
+        <v>2019</v>
       </c>
       <c r="F3">
-        <v>35000</v>
+        <v>16698</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J3">
-        <v>5461</v>
+        <v>1199</v>
       </c>
       <c r="K3">
-        <v>387.3</v>
+        <v>84</v>
       </c>
       <c r="L3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M3">
-        <v>8.1</v>
+        <v>23.84</v>
       </c>
       <c r="N3">
-        <v>29.5</v>
+        <v>5.85</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4">
-        <v>152</v>
+        <v>3263</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="E4">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="F4">
-        <v>35277</v>
+        <v>80000</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J4">
-        <v>5461</v>
+        <v>1248</v>
       </c>
       <c r="K4">
-        <v>362.9</v>
+        <v>74</v>
       </c>
       <c r="L4">
         <v>5</v>
       </c>
       <c r="M4">
-        <v>7.81</v>
+        <v>22.3</v>
       </c>
       <c r="N4">
-        <v>30</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5">
-        <v>589</v>
+        <v>3551</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E5">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="F5">
-        <v>47088</v>
+        <v>73000</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="J5">
-        <v>3498</v>
+        <v>1396</v>
       </c>
       <c r="K5">
-        <v>364.9</v>
+        <v>65</v>
       </c>
       <c r="L5">
         <v>5</v>
       </c>
       <c r="M5">
-        <v>10.13</v>
+        <v>14.4</v>
       </c>
       <c r="N5">
-        <v>19</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6">
-        <v>1930</v>
+        <v>319</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E6">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="F6">
-        <v>55000</v>
+        <v>138000</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J6">
-        <v>3498</v>
+        <v>1396</v>
       </c>
       <c r="K6">
-        <v>364.9</v>
+        <v>70</v>
       </c>
       <c r="L6">
         <v>5</v>
       </c>
       <c r="M6">
-        <v>10.13</v>
+        <v>17.1</v>
       </c>
       <c r="N6">
-        <v>9.99</v>
+        <v>1.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>